<commit_message>
fix bug when loading json to executer
</commit_message>
<xml_diff>
--- a/schedule2.xlsx
+++ b/schedule2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{2CB886C7-02C3-4763-9EF3-620FB0B81056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECADF7FE-33B8-432F-AD78-A989B15EDCA5}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="13_ncr:1_{2CB886C7-02C3-4763-9EF3-620FB0B81056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A07CBC4-6DFB-4EBE-A2BB-A92416FABDC6}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-3070" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -783,6 +783,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -794,12 +800,6 @@
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1318,8 +1318,8 @@
   <dimension ref="A1:BL31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <pane ySplit="6" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1372,107 +1372,107 @@
         <v>4</v>
       </c>
       <c r="B3" s="46"/>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="75"/>
-      <c r="E3" s="73">
+      <c r="D3" s="71"/>
+      <c r="E3" s="75">
         <f>DATE(2022,8,29)</f>
         <v>44802</v>
       </c>
-      <c r="F3" s="73"/>
+      <c r="F3" s="75"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="74" t="s">
+      <c r="C4" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="75"/>
+      <c r="D4" s="71"/>
       <c r="E4" s="7">
         <v>2</v>
       </c>
-      <c r="I4" s="70">
+      <c r="I4" s="72">
         <f>I5</f>
         <v>44809</v>
       </c>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
-      <c r="M4" s="71"/>
-      <c r="N4" s="71"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="70">
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="72">
         <f>P5</f>
         <v>44816</v>
       </c>
-      <c r="Q4" s="71"/>
-      <c r="R4" s="71"/>
-      <c r="S4" s="71"/>
-      <c r="T4" s="71"/>
-      <c r="U4" s="71"/>
-      <c r="V4" s="72"/>
-      <c r="W4" s="70">
+      <c r="Q4" s="73"/>
+      <c r="R4" s="73"/>
+      <c r="S4" s="73"/>
+      <c r="T4" s="73"/>
+      <c r="U4" s="73"/>
+      <c r="V4" s="74"/>
+      <c r="W4" s="72">
         <f>W5</f>
         <v>44823</v>
       </c>
-      <c r="X4" s="71"/>
-      <c r="Y4" s="71"/>
-      <c r="Z4" s="71"/>
-      <c r="AA4" s="71"/>
-      <c r="AB4" s="71"/>
-      <c r="AC4" s="72"/>
-      <c r="AD4" s="70">
+      <c r="X4" s="73"/>
+      <c r="Y4" s="73"/>
+      <c r="Z4" s="73"/>
+      <c r="AA4" s="73"/>
+      <c r="AB4" s="73"/>
+      <c r="AC4" s="74"/>
+      <c r="AD4" s="72">
         <f>AD5</f>
         <v>44830</v>
       </c>
-      <c r="AE4" s="71"/>
-      <c r="AF4" s="71"/>
-      <c r="AG4" s="71"/>
-      <c r="AH4" s="71"/>
-      <c r="AI4" s="71"/>
-      <c r="AJ4" s="72"/>
-      <c r="AK4" s="70">
+      <c r="AE4" s="73"/>
+      <c r="AF4" s="73"/>
+      <c r="AG4" s="73"/>
+      <c r="AH4" s="73"/>
+      <c r="AI4" s="73"/>
+      <c r="AJ4" s="74"/>
+      <c r="AK4" s="72">
         <f>AK5</f>
         <v>44837</v>
       </c>
-      <c r="AL4" s="71"/>
-      <c r="AM4" s="71"/>
-      <c r="AN4" s="71"/>
-      <c r="AO4" s="71"/>
-      <c r="AP4" s="71"/>
-      <c r="AQ4" s="72"/>
-      <c r="AR4" s="70">
+      <c r="AL4" s="73"/>
+      <c r="AM4" s="73"/>
+      <c r="AN4" s="73"/>
+      <c r="AO4" s="73"/>
+      <c r="AP4" s="73"/>
+      <c r="AQ4" s="74"/>
+      <c r="AR4" s="72">
         <f>AR5</f>
         <v>44844</v>
       </c>
-      <c r="AS4" s="71"/>
-      <c r="AT4" s="71"/>
-      <c r="AU4" s="71"/>
-      <c r="AV4" s="71"/>
-      <c r="AW4" s="71"/>
-      <c r="AX4" s="72"/>
-      <c r="AY4" s="70">
+      <c r="AS4" s="73"/>
+      <c r="AT4" s="73"/>
+      <c r="AU4" s="73"/>
+      <c r="AV4" s="73"/>
+      <c r="AW4" s="73"/>
+      <c r="AX4" s="74"/>
+      <c r="AY4" s="72">
         <f>AY5</f>
         <v>44851</v>
       </c>
-      <c r="AZ4" s="71"/>
-      <c r="BA4" s="71"/>
-      <c r="BB4" s="71"/>
-      <c r="BC4" s="71"/>
-      <c r="BD4" s="71"/>
-      <c r="BE4" s="72"/>
-      <c r="BF4" s="70">
+      <c r="AZ4" s="73"/>
+      <c r="BA4" s="73"/>
+      <c r="BB4" s="73"/>
+      <c r="BC4" s="73"/>
+      <c r="BD4" s="73"/>
+      <c r="BE4" s="74"/>
+      <c r="BF4" s="72">
         <f>BF5</f>
         <v>44858</v>
       </c>
-      <c r="BG4" s="71"/>
-      <c r="BH4" s="71"/>
-      <c r="BI4" s="71"/>
-      <c r="BJ4" s="71"/>
-      <c r="BK4" s="71"/>
-      <c r="BL4" s="72"/>
+      <c r="BG4" s="73"/>
+      <c r="BH4" s="73"/>
+      <c r="BI4" s="73"/>
+      <c r="BJ4" s="73"/>
+      <c r="BK4" s="73"/>
+      <c r="BL4" s="74"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="41" t="s">
@@ -3064,7 +3064,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="31">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E21" s="49">
         <f>E19</f>
@@ -3145,7 +3145,7 @@
         <v>3</v>
       </c>
       <c r="D22" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="49">
         <f>F21+1</f>
@@ -3226,7 +3226,7 @@
         <v>3</v>
       </c>
       <c r="D23" s="31">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="E23" s="49">
         <f>F21+1</f>
@@ -3707,17 +3707,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D28">
     <cfRule type="dataBar" priority="14">

</xml_diff>